<commit_message>
update loading task, README and TaskJob
</commit_message>
<xml_diff>
--- a/TaskJob.xlsx
+++ b/TaskJob.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BC41\capstone-project-airbnb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D69F7460-39BB-41EB-96B3-A38D30ACE930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D107C82-95BC-4DB2-914E-78766779C716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -177,7 +177,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,6 +214,12 @@
         <bgColor rgb="FFAEABAB"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFAEABAB"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -242,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -279,6 +285,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -514,7 +523,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
+      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -824,7 +833,9 @@
       <c r="G10" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="9"/>
+      <c r="H10" s="9">
+        <v>1</v>
+      </c>
       <c r="I10" s="12" t="s">
         <v>13</v>
       </c>
@@ -910,7 +921,7 @@
       <c r="G13" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="9"/>
+      <c r="H13" s="13"/>
       <c r="I13" s="12" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
update fix bug booking room and update task job
</commit_message>
<xml_diff>
--- a/TaskJob.xlsx
+++ b/TaskJob.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BC41\capstone-project-airbnb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D107C82-95BC-4DB2-914E-78766779C716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1203D3-0F70-4BE1-94A0-F19F46BD09AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="35">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>API trả về thiếu thông tin</t>
+  </si>
+  <si>
+    <t>Thiếu thêm, xóa, sửa</t>
+  </si>
+  <si>
+    <t>Chưa edit + update ảnh</t>
   </si>
 </sst>
 </file>
@@ -523,7 +529,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
+      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -893,11 +899,15 @@
       <c r="G12" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="9"/>
+      <c r="H12" s="9">
+        <v>0.5</v>
+      </c>
       <c r="I12" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="11"/>
+      <c r="J12" s="11" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -921,7 +931,9 @@
       <c r="G13" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="13"/>
+      <c r="H13" s="13">
+        <v>1</v>
+      </c>
       <c r="I13" s="12" t="s">
         <v>14</v>
       </c>
@@ -951,11 +963,15 @@
       <c r="G14" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="H14" s="9"/>
+      <c r="H14" s="9">
+        <v>0.25</v>
+      </c>
       <c r="I14" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="11"/>
+      <c r="J14" s="11" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
@@ -980,12 +996,14 @@
         <v>31</v>
       </c>
       <c r="H15" s="9">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="I15" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="J15" s="11"/>
+      <c r="J15" s="11" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="16" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">

</xml_diff>